<commit_message>
Pequeñas modificaciones al script
</commit_message>
<xml_diff>
--- a/Tablas BD.xlsx
+++ b/Tablas BD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RegistroWEB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6D24729-DA1A-4F48-BE9D-F481FA5B8879}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AA763F-B825-4C71-8C88-53C14DEDFF6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{12F7FFF0-2BDC-4865-B098-027C72E8D5F0}"/>
+    <workbookView xWindow="3375" yWindow="2775" windowWidth="15375" windowHeight="7875" xr2:uid="{12F7FFF0-2BDC-4865-B098-027C72E8D5F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
-  <si>
-    <t>Sugerencia BD registro empleados</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Empleado</t>
   </si>
@@ -121,6 +118,12 @@
   </si>
   <si>
     <t>Varchar 30</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Tablas de BD registro empleados</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -229,11 +232,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -245,6 +261,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F27713-4F5E-47F3-BC74-27CE86AA01ED}">
   <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,155 +598,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
+      <c r="H9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>